<commit_message>
Rerunning and recording runs of models with correctly initialised weights (early stopping and otherwise)
</commit_message>
<xml_diff>
--- a/Dyck 1 Counter/Dyck1_Counter_6_early_stopping_Softmax_BCE.xlsx
+++ b/Dyck 1 Counter/Dyck1_Counter_6_early_stopping_Softmax_BCE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>epochs</t>
   </si>
@@ -82,59 +82,29 @@
     <t>epoch incorrect guesses</t>
   </si>
   <si>
-    <t>[-0.01051079  1.008067  ]</t>
-  </si>
-  <si>
-    <t>-0.012308901</t>
-  </si>
-  <si>
-    <t>[ 1.0008826 -0.0080965]</t>
-  </si>
-  <si>
-    <t>-0.0072139204</t>
-  </si>
-  <si>
-    <t>[1.0076953 0.9936731]</t>
-  </si>
-  <si>
-    <t>-0.0065105576</t>
-  </si>
-  <si>
-    <t>[1.0006428 1.0027208]</t>
-  </si>
-  <si>
-    <t>-0.0022227052</t>
-  </si>
-  <si>
-    <t>[-1.010414   0.9905151]</t>
-  </si>
-  <si>
-    <t>-0.008878276</t>
-  </si>
-  <si>
-    <t>[1.0008777]</t>
-  </si>
-  <si>
-    <t>-0.008865433</t>
-  </si>
-  <si>
-    <t>[ 0.9894487 -1.0161918]</t>
-  </si>
-  <si>
-    <t>-0.005679437</t>
-  </si>
-  <si>
-    <t>[1.0055637 1.015092 ]</t>
-  </si>
-  <si>
-    <t>-0.016743124</t>
-  </si>
-  <si>
-    <t>[[ 1.0026414  1.0004418]
- [-1.0026414 -1.0004418]]</t>
-  </si>
-  <si>
-    <t>[-0.01412299  1.014123  ]</t>
+    <t>[0. 1.]</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>[1. 0.]</t>
+  </si>
+  <si>
+    <t>[1. 1.]</t>
+  </si>
+  <si>
+    <t>[-1.  1.]</t>
+  </si>
+  <si>
+    <t>[1.]</t>
+  </si>
+  <si>
+    <t>[ 1. -1.]</t>
+  </si>
+  <si>
+    <t>[[ 1.  1.]
+ [-1. -1.]]</t>
   </si>
   <si>
     <t>[]</t>
@@ -586,58 +556,58 @@
         <v>24</v>
       </c>
       <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="U2">
-        <v>0.2256610493293939</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>100</v>
       </c>
       <c r="W2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>